<commit_message>
Schematic Updates: Added Brake Part
auxlary power design added

Co-Authored-By: KaanDemirkoparan <57269134+KaanDemirkoparan@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/[05]Docs/BOM List.xlsx
+++ b/[05]Docs/BOM List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaand\Desktop\Okul\EE463-Hardware-Project-2025\[05]Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\4.sınıf 1. dönem\EE463\EE463-Hardware-Project-2025\[05]Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417B8E7C-6F98-4195-A067-79F4E165F01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07FFBA2A-C3CC-487B-ACE3-611C28EAB3EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -1086,20 +1086,20 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="64" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
@@ -1358,7 +1358,7 @@
       </c>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
@@ -1416,7 +1416,7 @@
       </c>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>28</v>
       </c>
@@ -1445,7 +1445,7 @@
       </c>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>30</v>
       </c>
@@ -1474,7 +1474,7 @@
       </c>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -1503,7 +1503,7 @@
       </c>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>34</v>
       </c>
@@ -1532,7 +1532,7 @@
       </c>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>61</v>
       </c>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>62</v>
       </c>
@@ -1590,7 +1590,7 @@
       </c>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>60</v>
       </c>
@@ -1619,7 +1619,7 @@
       </c>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>64</v>
       </c>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>39</v>
       </c>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="I20" s="6"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>63</v>
       </c>
@@ -1706,7 +1706,7 @@
       </c>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>66</v>
       </c>
@@ -1735,7 +1735,7 @@
       </c>
       <c r="I22" s="6"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>42</v>
       </c>
@@ -1764,7 +1764,7 @@
       </c>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>44</v>
       </c>
@@ -1793,7 +1793,7 @@
       </c>
       <c r="I24" s="6"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>45</v>
       </c>
@@ -1822,7 +1822,7 @@
       </c>
       <c r="I25" s="6"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>51</v>
       </c>
@@ -1841,7 +1841,7 @@
       </c>
       <c r="I26" s="6"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>52</v>
       </c>
@@ -1870,7 +1870,7 @@
       </c>
       <c r="I27" s="6"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>53</v>
       </c>
@@ -1899,7 +1899,7 @@
       </c>
       <c r="I28" s="6"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>54</v>
       </c>
@@ -1928,7 +1928,7 @@
       </c>
       <c r="I29" s="6"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>55</v>
       </c>
@@ -1957,7 +1957,7 @@
       </c>
       <c r="I30" s="6"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>67</v>
       </c>
@@ -1989,7 +1989,7 @@
       </c>
       <c r="I31" s="6"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>70</v>
       </c>
@@ -2021,7 +2021,7 @@
       </c>
       <c r="I32" s="6"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2032,7 +2032,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="6"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2043,7 +2043,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="6"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2054,7 +2054,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="6"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2065,7 +2065,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>47</v>
       </c>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="I37" s="13"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>56</v>
       </c>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="I38" s="13"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
         <v>57</v>
       </c>

</xml_diff>